<commit_message>
bigger icons, better text
</commit_message>
<xml_diff>
--- a/docs/translations.xlsx
+++ b/docs/translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\IdeaProjects\neoCAPTCHA\frontend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF07278-6D96-4CD9-8D8B-76FDEEB9E0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27A071B-D900-4DEB-A104-DFAE5DA63CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,9 +135,6 @@
     <t>Klicke beim Signalton!</t>
   </si>
   <si>
-    <t>Click when you hear a signal!</t>
-  </si>
-  <si>
     <t>Solve the CAPTCHA!</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>CODE</t>
+  </si>
+  <si>
+    <t>Click at the signal tone!</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +557,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
@@ -618,7 +618,7 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -629,10 +629,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
         <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -640,10 +640,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -651,10 +651,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
         <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -662,10 +662,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -673,10 +673,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -695,10 +695,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -706,10 +706,10 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
improved ui, option: visualOnDesktop
</commit_message>
<xml_diff>
--- a/docs/translations.xlsx
+++ b/docs/translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\IdeaProjects\neoCAPTCHA\frontend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF07278-6D96-4CD9-8D8B-76FDEEB9E0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98330AAC-5947-4F77-B84E-403427ABFAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,9 +135,6 @@
     <t>Klicke beim Signalton!</t>
   </si>
   <si>
-    <t>Click when you hear a signal!</t>
-  </si>
-  <si>
     <t>Solve the CAPTCHA!</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>CODE</t>
+  </si>
+  <si>
+    <t>Click at the signal tone!</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +557,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
@@ -618,7 +618,7 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -629,10 +629,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
         <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -640,10 +640,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -651,10 +651,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
         <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -662,10 +662,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -673,10 +673,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -695,10 +695,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -706,10 +706,10 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
more compact ui, bg fills up when shaking
</commit_message>
<xml_diff>
--- a/docs/translations.xlsx
+++ b/docs/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\IdeaProjects\neoCAPTCHA\frontend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD68EE1-1B3E-4966-B020-F0EA15FE6E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C140EB12-5219-4484-9896-A477BCA396B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>step_1</t>
   </si>
@@ -141,24 +141,12 @@
     <t>Löse das CAPTCHA!</t>
   </si>
   <si>
-    <t>Angedeutetes Viereck:</t>
-  </si>
-  <si>
-    <t>Implied Square:</t>
-  </si>
-  <si>
     <t>Mark the missing corner!</t>
   </si>
   <si>
     <t>Markiere die fehlende Ecke!</t>
   </si>
   <si>
-    <t>Neon-Form:</t>
-  </si>
-  <si>
-    <t>Neon Shape:</t>
-  </si>
-  <si>
     <t>Welche Form siehst du?</t>
   </si>
   <si>
@@ -181,6 +169,27 @@
   </si>
   <si>
     <t>Click after the sound cue!</t>
+  </si>
+  <si>
+    <t>step_2_motion</t>
+  </si>
+  <si>
+    <t>Shake your phone!</t>
+  </si>
+  <si>
+    <t>Schüttel dein Handy!</t>
+  </si>
+  <si>
+    <t>Implied Square</t>
+  </si>
+  <si>
+    <t>Angedeutetes Viereck</t>
+  </si>
+  <si>
+    <t>Neon-Form</t>
+  </si>
+  <si>
+    <t>Neon Shape</t>
   </si>
 </sst>
 </file>
@@ -535,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +566,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
@@ -618,7 +627,7 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -626,122 +635,133 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
info when too many requests
</commit_message>
<xml_diff>
--- a/docs/translations.xlsx
+++ b/docs/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\IdeaProjects\neoCAPTCHA\frontend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C140EB12-5219-4484-9896-A477BCA396B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7FA34A-D7A1-489F-AB49-DD63F2FD9F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>step_1</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>Neon Shape</t>
+  </si>
+  <si>
+    <t>too_many_requests</t>
+  </si>
+  <si>
+    <t>Please wait a minute before trying again.</t>
+  </si>
+  <si>
+    <t>Bitte warte eine Minute, bevor du es erneut versuchst.</t>
   </si>
 </sst>
 </file>
@@ -544,17 +553,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
+    <col min="3" max="3" width="51" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
     <col min="5" max="5" width="30.28515625" customWidth="1"/>
     <col min="6" max="6" width="27.5703125" customWidth="1"/>
@@ -701,67 +710,78 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>